<commit_message>
Update the script and requirement files
</commit_message>
<xml_diff>
--- a/combined_results.xlsx
+++ b/combined_results.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E59"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,11 +464,11 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>GKA 123X</t>
+          <t>GKA 917K</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>233</v>
+        <v>1628</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -476,20 +476,20 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>45</v>
+        <v>56.68</v>
       </c>
       <c r="E2" t="n">
-        <v>8721</v>
+        <v>10701.2</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>GKA 123X</t>
+          <t>GKA 917K</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1957</v>
+        <v>3679</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -497,20 +497,20 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>37.75</v>
+        <v>58</v>
       </c>
       <c r="E3" t="n">
-        <v>7516</v>
+        <v>11008</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>GKA 123X</t>
+          <t>GKA 917K</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>3300</v>
+        <v>3944</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -518,20 +518,20 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="E4" t="n">
-        <v>10465</v>
+        <v>11008</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>GKA 123X</t>
+          <t>GKA 917K</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>3507</v>
+        <v>4956</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -539,83 +539,83 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>45.96</v>
+        <v>60</v>
       </c>
       <c r="E5" t="n">
-        <v>8907</v>
+        <v>11328</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>GKA 123X</t>
+          <t>KAN 670U</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>5002</v>
+        <v>1495</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>LUBRICANTS</t>
+          <t>PREMIUM</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>58.01</v>
       </c>
       <c r="E6" t="n">
-        <v>4000</v>
+        <v>11010.3</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>GKA 917K</t>
+          <t>KAW 135Z</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1002</v>
+        <v>1492</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>PREMIUM</t>
+          <t>DIESEL</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>45.9</v>
+        <v>170.52</v>
       </c>
       <c r="E7" t="n">
-        <v>8895.4</v>
+        <v>29262</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>GKA 917K</t>
+          <t>KAW 135Z</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2706</v>
+        <v>1546</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>PREMIUM</t>
+          <t>PUNCTURE</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>60</v>
+        <v>1</v>
       </c>
       <c r="E8" t="n">
-        <v>11946</v>
+        <v>200</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>KAL 980U</t>
+          <t>KAW 135Z</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>6581</v>
+        <v>2950</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -623,41 +623,41 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>215.09</v>
+        <v>111.46</v>
       </c>
       <c r="E9" t="n">
-        <v>40931.7</v>
+        <v>19293</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>KAL 980U</t>
+          <t>KAY 040V</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>6582</v>
+        <v>1428</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>LUBRICANTS</t>
+          <t>PREMIUM</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>4750</v>
+        <v>43.52</v>
       </c>
       <c r="E10" t="n">
-        <v>4750</v>
+        <v>8260.1</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>KAN 670U</t>
+          <t>KAY 040V</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>879</v>
+        <v>3940</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -665,20 +665,20 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>52.01</v>
+        <v>58</v>
       </c>
       <c r="E11" t="n">
-        <v>10355.2</v>
+        <v>11008</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>KAN 670U</t>
+          <t>KAY 040V</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>963</v>
+        <v>4116</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -686,62 +686,62 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>58</v>
+        <v>47.44</v>
       </c>
       <c r="E12" t="n">
-        <v>11240.4</v>
+        <v>9005</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>KAW 135Z</t>
+          <t>KAY 040V</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>970</v>
+        <v>4378</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>DIESEL</t>
+          <t>PREMIUM</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>126.14</v>
+        <v>58</v>
       </c>
       <c r="E13" t="n">
-        <v>22743.1</v>
+        <v>10950</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>KAW 135Z</t>
+          <t>KAY 040V</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>6052</v>
+        <v>4379</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>DIESEL</t>
+          <t>LUBRICANTS</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>105.58</v>
+        <v>1</v>
       </c>
       <c r="E14" t="n">
-        <v>20040</v>
+        <v>2650</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>KAY 040V</t>
+          <t>KAY 298V</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>388</v>
+        <v>4430</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -749,20 +749,20 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E15" t="n">
-        <v>11946</v>
+        <v>10572</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>KAY 040V</t>
+          <t>KBB 417S</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>426</v>
+        <v>1430</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -770,20 +770,20 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>58</v>
+        <v>18.6</v>
       </c>
       <c r="E16" t="n">
-        <v>11547</v>
+        <v>3530.3</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>KAY 040V</t>
+          <t>KBB 770S</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>1912</v>
+        <v>5165</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -791,83 +791,83 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>58.06</v>
+        <v>54.89</v>
       </c>
       <c r="E17" t="n">
-        <v>11559</v>
+        <v>10363</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>KAY 040V</t>
+          <t>KBJ 420U</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>3103</v>
+        <v>3941</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>PREMIUM</t>
+          <t>DIESEL</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>54.29</v>
+        <v>62</v>
       </c>
       <c r="E18" t="n">
-        <v>10809</v>
+        <v>10732</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>KAY 040V</t>
+          <t>KBJ 420U</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>3235</v>
+        <v>4234</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>PREMIUM</t>
+          <t>DIESEL</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="E19" t="n">
-        <v>11046</v>
+        <v>5985</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>KAY 040V</t>
+          <t>KBJ 420U</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>3451</v>
+        <v>4319</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>PREMIUM</t>
+          <t>DIESEL</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>48.38</v>
+        <v>58</v>
       </c>
       <c r="E20" t="n">
-        <v>9377</v>
+        <v>9994</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>KAY 040V</t>
+          <t>KBJ 420U</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>5960</v>
+        <v>4504</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -875,83 +875,83 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E21" t="n">
-        <v>2260</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>KAY 040V</t>
+          <t>KBQ 254D</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>6177</v>
+        <v>1040</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>LUBRICANTS</t>
+          <t>DIESEL</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>4</v>
+        <v>56.91</v>
       </c>
       <c r="E22" t="n">
-        <v>2280</v>
+        <v>9851.1</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>KAY 040V</t>
+          <t>KBQ 254D</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>6258</v>
+        <v>1681</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>PREMIUM</t>
+          <t>DIESEL</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>41.7</v>
+        <v>68</v>
       </c>
       <c r="E23" t="n">
-        <v>8305.299999999999</v>
+        <v>11668</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>KAY 040V</t>
+          <t>KBR 791U</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>6259</v>
+        <v>1608</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>LUBRICANTS</t>
+          <t>PREMIUM</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>0.01</v>
+        <v>47.12</v>
       </c>
       <c r="E24" t="n">
-        <v>870</v>
+        <v>8896.299999999999</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>KAY 298V</t>
+          <t>KBZ 546D</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>13</v>
+        <v>1115</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -959,20 +959,20 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>44.46</v>
+        <v>8.44</v>
       </c>
       <c r="E25" t="n">
-        <v>8852</v>
+        <v>1602</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>KAY 298V</t>
+          <t>KBZ 546D</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>3681</v>
+        <v>1482</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
@@ -980,20 +980,20 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>41.21</v>
+        <v>8.550000000000001</v>
       </c>
       <c r="E26" t="n">
-        <v>8217.299999999999</v>
+        <v>1622.8</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>KAY 298V</t>
+          <t>KBZ 546D</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>6473</v>
+        <v>1545</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -1001,41 +1001,41 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>36.36</v>
+        <v>8.609999999999999</v>
       </c>
       <c r="E27" t="n">
-        <v>7046.6</v>
+        <v>1625.6</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>KBB 417S</t>
+          <t>KBZ 546D</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>2851</v>
+        <v>1690</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>LUBRICANTS</t>
+          <t>PREMIUM</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>1</v>
+        <v>7.11</v>
       </c>
       <c r="E28" t="n">
-        <v>2450</v>
+        <v>1342.4</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>KBB 770S</t>
+          <t>KBZ 546D</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>144</v>
+        <v>1913</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
@@ -1043,62 +1043,62 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>68.7</v>
+        <v>4.27</v>
       </c>
       <c r="E29" t="n">
-        <v>13314</v>
+        <v>807</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>KBB 770S</t>
+          <t>KCD 388 G</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>2921</v>
+        <v>5795</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>PREMIUM</t>
+          <t>DIESEL</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>46.32</v>
+        <v>78</v>
       </c>
       <c r="E30" t="n">
-        <v>9223</v>
+        <v>13501</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>KBB 770S</t>
+          <t>KCD 388 G</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>3800</v>
+        <v>9314</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>PREMIUM</t>
+          <t>DIESEL</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>68.45999999999999</v>
+        <v>77.90000000000001</v>
       </c>
       <c r="E31" t="n">
-        <v>13267</v>
+        <v>13235.1</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>KBJ 420U</t>
+          <t>KCD 388 G</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>53</v>
+        <v>9728</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -1106,20 +1106,20 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="E32" t="n">
-        <v>11539.2</v>
+        <v>12630</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>KBQ 254D</t>
+          <t>KCD 390 G</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>1</v>
+        <v>3943</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -1127,532 +1127,191 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>62.25</v>
+        <v>76</v>
       </c>
       <c r="E33" t="n">
-        <v>11846.8</v>
+        <v>13155</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>KBR 791U</t>
+          <t>KCD 390 G</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>951</v>
+        <v>4357</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>PREMIUM</t>
+          <t>DIESEL</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>42.87</v>
+        <v>75.8</v>
       </c>
       <c r="E34" t="n">
-        <v>8308.299999999999</v>
+        <v>13091</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>KBR 791U</t>
+          <t>KCD 390 G</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>974</v>
+        <v>4359</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>PREMIUM</t>
+          <t>PUNCTURE</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>40.83</v>
+        <v>1</v>
       </c>
       <c r="E35" t="n">
-        <v>7912.9</v>
+        <v>200</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>KBR 791U</t>
+          <t>KCD 390 G</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>2644</v>
+        <v>4994</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>PREMIUM</t>
+          <t>DIESEL</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>53</v>
+        <v>56.99</v>
       </c>
       <c r="E36" t="n">
-        <v>10552</v>
+        <v>9763</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>KBZ 182D</t>
+          <t>KCH 905Q</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>64</v>
+        <v>1464</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>DIESEL</t>
+          <t>PREMIUM</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>74.95999999999999</v>
+        <v>36.7</v>
       </c>
       <c r="E37" t="n">
-        <v>13515</v>
+        <v>6965.7</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>KBZ 182D</t>
+          <t>KCH 905Q</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>3301</v>
+        <v>2041</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>DIESEL</t>
+          <t>PREMIUM</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>94.5</v>
+        <v>32.69</v>
       </c>
       <c r="E38" t="n">
-        <v>17038</v>
+        <v>6171.9</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>KBZ 182D</t>
+          <t>KCT846Y</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>8528</v>
+        <v>3928</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>LUBRICANTS</t>
+          <t>DIESEL</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>5</v>
+        <v>108.89</v>
       </c>
       <c r="E39" t="n">
-        <v>2650</v>
+        <v>18848</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>KBZ 546D</t>
+          <t>KCT846Y</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>5657</v>
+        <v>4598</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>PREMIUM</t>
+          <t>DIESEL</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>10</v>
+        <v>130.55</v>
       </c>
       <c r="E40" t="n">
-        <v>1991</v>
+        <v>22402</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>KBZ 546D</t>
+          <t>KCT846Y</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>5670</v>
+        <v>4989</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>LUBRICANTS</t>
+          <t>DIESEL</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>1</v>
+        <v>142</v>
       </c>
       <c r="E41" t="n">
-        <v>500</v>
+        <v>24367</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>KBZ 546D</t>
-        </is>
-      </c>
-      <c r="B42" t="n">
-        <v>6375</v>
-      </c>
+      <c r="A42" t="inlineStr"/>
+      <c r="B42" t="inlineStr"/>
       <c r="C42" t="inlineStr">
         <is>
-          <t>PREMIUM</t>
-        </is>
-      </c>
-      <c r="D42" t="n">
-        <v>9.42</v>
-      </c>
+          <t>Client fee</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr"/>
       <c r="E42" t="n">
-        <v>1825.6</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>KBZ 546D</t>
-        </is>
-      </c>
-      <c r="B43" t="n">
-        <v>6555</v>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>PREMIUM</t>
-        </is>
-      </c>
-      <c r="D43" t="n">
-        <v>8.73</v>
-      </c>
-      <c r="E43" t="n">
-        <v>1691.9</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>KCD 388 G</t>
-        </is>
-      </c>
-      <c r="B44" t="n">
-        <v>6880</v>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>DIESEL</t>
-        </is>
-      </c>
-      <c r="D44" t="n">
-        <v>79</v>
-      </c>
-      <c r="E44" t="n">
-        <v>14788.8</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>KCD 388 G</t>
-        </is>
-      </c>
-      <c r="B45" t="n">
-        <v>7212</v>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>DIESEL</t>
-        </is>
-      </c>
-      <c r="D45" t="n">
-        <v>78</v>
-      </c>
-      <c r="E45" t="n">
-        <v>13821.6</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>KCD 390 G</t>
-        </is>
-      </c>
-      <c r="B46" t="n">
-        <v>1771</v>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>DIESEL</t>
-        </is>
-      </c>
-      <c r="D46" t="n">
-        <v>72.02</v>
-      </c>
-      <c r="E46" t="n">
-        <v>12985.2</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>KCD 390 G</t>
-        </is>
-      </c>
-      <c r="B47" t="n">
-        <v>2850</v>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>DIESEL</t>
-        </is>
-      </c>
-      <c r="D47" t="n">
-        <v>45.2</v>
-      </c>
-      <c r="E47" t="n">
-        <v>8601</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>KCD 390 G</t>
-        </is>
-      </c>
-      <c r="B48" t="n">
-        <v>3654</v>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>DIESEL</t>
-        </is>
-      </c>
-      <c r="D48" t="n">
-        <v>71.05</v>
-      </c>
-      <c r="E48" t="n">
-        <v>12810</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>KCD 390 G</t>
-        </is>
-      </c>
-      <c r="B49" t="n">
-        <v>3902</v>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>DIESEL</t>
-        </is>
-      </c>
-      <c r="D49" t="n">
-        <v>67.34</v>
-      </c>
-      <c r="E49" t="n">
-        <v>12605.2</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>KCD 390 G</t>
-        </is>
-      </c>
-      <c r="B50" t="n">
-        <v>3903</v>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>LUBRICANTS</t>
-        </is>
-      </c>
-      <c r="D50" t="n">
-        <v>1</v>
-      </c>
-      <c r="E50" t="n">
-        <v>1100</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>KCD 390 G</t>
-        </is>
-      </c>
-      <c r="B51" t="n">
-        <v>4099</v>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>DIESEL</t>
-        </is>
-      </c>
-      <c r="D51" t="n">
-        <v>43.52</v>
-      </c>
-      <c r="E51" t="n">
-        <v>8146.5</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>KCH 905Q</t>
-        </is>
-      </c>
-      <c r="B52" t="n">
-        <v>6373</v>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>PREMIUM</t>
-        </is>
-      </c>
-      <c r="D52" t="n">
-        <v>30.86</v>
-      </c>
-      <c r="E52" t="n">
-        <v>5980.7</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>KCT846Y</t>
-        </is>
-      </c>
-      <c r="B53" t="n">
-        <v>363</v>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>DIESEL</t>
-        </is>
-      </c>
-      <c r="D53" t="n">
-        <v>112</v>
-      </c>
-      <c r="E53" t="n">
-        <v>20967</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>KCT846Y</t>
-        </is>
-      </c>
-      <c r="B54" t="n">
-        <v>2318</v>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>DIESEL</t>
-        </is>
-      </c>
-      <c r="D54" t="n">
-        <v>144.31</v>
-      </c>
-      <c r="E54" t="n">
-        <v>27462</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>KCT846Y</t>
-        </is>
-      </c>
-      <c r="B55" t="n">
-        <v>3901</v>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>DIESEL</t>
-        </is>
-      </c>
-      <c r="D55" t="n">
-        <v>144.25</v>
-      </c>
-      <c r="E55" t="n">
-        <v>27003.6</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>KCT846Y</t>
-        </is>
-      </c>
-      <c r="B56" t="n">
-        <v>4098</v>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>DIESEL</t>
-        </is>
-      </c>
-      <c r="D56" t="n">
-        <v>24.4</v>
-      </c>
-      <c r="E56" t="n">
-        <v>4567</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="inlineStr"/>
-      <c r="B57" t="inlineStr"/>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>Client fee</t>
-        </is>
-      </c>
-      <c r="D57" t="inlineStr"/>
-      <c r="E57" t="n">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="inlineStr"/>
-      <c r="B58" t="inlineStr"/>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>Client fee</t>
-        </is>
-      </c>
-      <c r="D58" t="inlineStr"/>
-      <c r="E58" t="n">
         <v>1000</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="inlineStr"/>
-      <c r="B59" t="inlineStr"/>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>Client fee</t>
-        </is>
-      </c>
-      <c r="D59" t="inlineStr"/>
-      <c r="E59" t="n">
-        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -1666,7 +1325,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1699,25 +1358,25 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>GKA 123X</t>
+          <t>GKA 917K</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>LUBRICANTS</t>
+          <t>PREMIUM</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>232.68</v>
       </c>
       <c r="D2" t="n">
-        <v>4000</v>
+        <v>44045.2</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>GKA 123X</t>
+          <t>KAN 670U</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -1726,52 +1385,52 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>182.71</v>
+        <v>58.01</v>
       </c>
       <c r="D3" t="n">
-        <v>35609</v>
+        <v>11010.3</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>GKA 917K</t>
+          <t>KAW 135Z</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>PREMIUM</t>
+          <t>DIESEL</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>105.9</v>
+        <v>281.98</v>
       </c>
       <c r="D4" t="n">
-        <v>20841.4</v>
+        <v>48555</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>KAL 980U</t>
+          <t>KAW 135Z</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>DIESEL</t>
+          <t>PUNCTURE</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>215.09</v>
+        <v>1</v>
       </c>
       <c r="D5" t="n">
-        <v>40931.7</v>
+        <v>200</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>KAL 980U</t>
+          <t>KAY 040V</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -1780,16 +1439,16 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>4750</v>
+        <v>1</v>
       </c>
       <c r="D6" t="n">
-        <v>4750</v>
+        <v>2650</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>KAN 670U</t>
+          <t>KAY 040V</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -1798,52 +1457,52 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>110.01</v>
+        <v>206.96</v>
       </c>
       <c r="D7" t="n">
-        <v>21595.6</v>
+        <v>39223.1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>KAW 135Z</t>
+          <t>KAY 298V</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>DIESEL</t>
+          <t>PREMIUM</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>231.72</v>
+        <v>56</v>
       </c>
       <c r="D8" t="n">
-        <v>42783.1</v>
+        <v>10572</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>KAY 040V</t>
+          <t>KBB 417S</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>LUBRICANTS</t>
+          <t>PREMIUM</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>8.01</v>
+        <v>18.6</v>
       </c>
       <c r="D9" t="n">
-        <v>5410</v>
+        <v>3530.3</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>KAY 040V</t>
+          <t>KBB 770S</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1852,34 +1511,34 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>377.43</v>
+        <v>54.89</v>
       </c>
       <c r="D10" t="n">
-        <v>74589.3</v>
+        <v>10363</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>KAY 298V</t>
+          <t>KBJ 420U</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>PREMIUM</t>
+          <t>DIESEL</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>122.03</v>
+        <v>155</v>
       </c>
       <c r="D11" t="n">
-        <v>24115.9</v>
+        <v>26711</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>KBB 417S</t>
+          <t>KBJ 420U</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -1888,88 +1547,88 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D12" t="n">
-        <v>2450</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>KBB 770S</t>
+          <t>KBQ 254D</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>PREMIUM</t>
+          <t>DIESEL</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>183.48</v>
+        <v>124.91</v>
       </c>
       <c r="D13" t="n">
-        <v>35804</v>
+        <v>21519.1</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>KBJ 420U</t>
+          <t>KBR 791U</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>DIESEL</t>
+          <t>PREMIUM</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>64</v>
+        <v>47.12</v>
       </c>
       <c r="D14" t="n">
-        <v>11539.2</v>
+        <v>8896.299999999999</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>KBQ 254D</t>
+          <t>KBZ 546D</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>DIESEL</t>
+          <t>PREMIUM</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>62.25</v>
+        <v>36.98</v>
       </c>
       <c r="D15" t="n">
-        <v>11846.8</v>
+        <v>6999.8</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>KBR 791U</t>
+          <t>KCD 388 G</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>PREMIUM</t>
+          <t>DIESEL</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>136.7</v>
+        <v>230.9</v>
       </c>
       <c r="D16" t="n">
-        <v>26773.2</v>
+        <v>39366.1</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>KBZ 182D</t>
+          <t>KCD 390 G</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1978,154 +1637,64 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>169.46</v>
+        <v>208.79</v>
       </c>
       <c r="D17" t="n">
-        <v>30553</v>
+        <v>36009</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>KBZ 182D</t>
+          <t>KCD 390 G</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>LUBRICANTS</t>
+          <t>PUNCTURE</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D18" t="n">
-        <v>2650</v>
+        <v>200</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>KBZ 546D</t>
+          <t>KCH 905Q</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>LUBRICANTS</t>
+          <t>PREMIUM</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>1</v>
+        <v>69.39</v>
       </c>
       <c r="D19" t="n">
-        <v>500</v>
+        <v>13137.6</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>KBZ 546D</t>
+          <t>KCT846Y</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>PREMIUM</t>
+          <t>DIESEL</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>28.15</v>
+        <v>381.44</v>
       </c>
       <c r="D20" t="n">
-        <v>5508.5</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>KCD 388 G</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>DIESEL</t>
-        </is>
-      </c>
-      <c r="C21" t="n">
-        <v>157</v>
-      </c>
-      <c r="D21" t="n">
-        <v>28610.4</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>KCD 390 G</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>DIESEL</t>
-        </is>
-      </c>
-      <c r="C22" t="n">
-        <v>299.13</v>
-      </c>
-      <c r="D22" t="n">
-        <v>55147.9</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>KCD 390 G</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>LUBRICANTS</t>
-        </is>
-      </c>
-      <c r="C23" t="n">
-        <v>1</v>
-      </c>
-      <c r="D23" t="n">
-        <v>1100</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>KCH 905Q</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>PREMIUM</t>
-        </is>
-      </c>
-      <c r="C24" t="n">
-        <v>30.86</v>
-      </c>
-      <c r="D24" t="n">
-        <v>5980.7</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>KCT846Y</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>DIESEL</t>
-        </is>
-      </c>
-      <c r="C25" t="n">
-        <v>424.96</v>
-      </c>
-      <c r="D25" t="n">
-        <v>79999.60000000001</v>
+        <v>65617</v>
       </c>
     </row>
   </sheetData>

</xml_diff>